<commit_message>
Set one of the applications to contested
</commit_message>
<xml_diff>
--- a/3-Certificates.xlsx
+++ b/3-Certificates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Library/Mobile Documents/com~apple~CloudDocs/Documents/Study/NMIT/SDV602/DM Digger/DM-Digger---1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72AF880D-360D-3E42-B5A8-9D2B2C8F9379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D2CDE0-DFBC-6348-B4B6-165A62C8B511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Application Type</t>
   </si>
@@ -116,6 +116,9 @@
   <si>
     <t>Alcohol Regulatory and Licensing Authority: Manager Certificates Register
 Active Certificates 2019-2022</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -477,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD188"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -618,7 +621,7 @@
         <v>4</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="M4" s="1"/>
     </row>

</xml_diff>